<commit_message>
some fixes with encoding
</commit_message>
<xml_diff>
--- a/input/names/names.xlsx
+++ b/input/names/names.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -21,26 +21,33 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Иванов Юрий Петрович</t>
+    <t>Жуков Александр Аркадьевич</t>
   </si>
   <si>
-    <t>Петров Александр Олегович</t>
+    <t>Жуков Дмитрий Алексеевич</t>
   </si>
   <si>
-    <t>Кузьмин Геннадий Викторович</t>
+    <t>Жуков Никита Юрьевич</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -51,7 +58,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -59,12 +66,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -348,27 +373,27 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.7265625" customWidth="1"/>
+    <col min="1" max="1" width="56.7109375" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>